<commit_message>
add callgrind info and hide files
</commit_message>
<xml_diff>
--- a/opt_results.xlsx
+++ b/opt_results.xlsx
@@ -56,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -93,7 +93,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1:AA33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1251,12 +1251,12 @@
         <v>0.25686299999999995</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" ref="C14:O14" si="0">AVERAGE(C3:C12)</f>
+        <f t="shared" ref="C14" si="0">AVERAGE(C3:C12)</f>
         <v>0.26692649999999996</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2">
-        <f t="shared" ref="E14:Q14" si="1">AVERAGE(E3:E12)</f>
+        <f t="shared" ref="E14:G14" si="1">AVERAGE(E3:E12)</f>
         <v>0.36045550000000004</v>
       </c>
       <c r="F14" s="2">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2">
-        <f t="shared" ref="I14:U14" si="2">AVERAGE(I3:I12)</f>
+        <f t="shared" ref="I14:K14" si="2">AVERAGE(I3:I12)</f>
         <v>0.52361460000000004</v>
       </c>
       <c r="J14" s="2">
@@ -1282,7 +1282,7 @@
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2">
-        <f t="shared" ref="M14:W14" si="3">AVERAGE(M3:M12)</f>
+        <f t="shared" ref="M14:O14" si="3">AVERAGE(M3:M12)</f>
         <v>1.4368234</v>
       </c>
       <c r="N14" s="2">
@@ -1308,7 +1308,7 @@
       </c>
       <c r="T14" s="2"/>
       <c r="U14" s="2">
-        <f t="shared" ref="T14:AA14" si="4">AVERAGE(U3:U12)</f>
+        <f t="shared" ref="U14:AA14" si="4">AVERAGE(U3:U12)</f>
         <v>0.32067279999999998</v>
       </c>
       <c r="V14" s="2">
@@ -1386,7 +1386,7 @@
         <v>1.3531782406675725</v>
       </c>
       <c r="S15" s="2">
-        <f t="shared" ref="S15:T15" si="12">C14/S14</f>
+        <f t="shared" ref="S15" si="12">C14/S14</f>
         <v>1.4061936972532161</v>
       </c>
       <c r="T15" s="2"/>
@@ -1395,7 +1395,7 @@
         <v>1.5914932604199676</v>
       </c>
       <c r="V15" s="2">
-        <f t="shared" ref="V15:AA15" si="13">B14/V14</f>
+        <f t="shared" ref="V15:W15" si="13">B14/V14</f>
         <v>1.4762792862951772</v>
       </c>
       <c r="W15" s="2">
@@ -1469,7 +1469,7 @@
         <v>1.3968944590195027</v>
       </c>
       <c r="S16" s="2">
-        <f t="shared" ref="S16:T16" si="21">G14/S14</f>
+        <f t="shared" ref="S16" si="21">G14/S14</f>
         <v>1.3926589120333788</v>
       </c>
       <c r="T16" s="2"/>

</xml_diff>